<commit_message>
Adds services for budgets and categories
</commit_message>
<xml_diff>
--- a/Docs/Breeze BRAID Log.xlsx
+++ b/Docs/Breeze BRAID Log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sean.kelley\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sean.kelley\source\repos\Breeze\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8D29CE-442D-49C1-8E1E-87BAD2254878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA13D2A-E28D-4E4A-AEC5-BE020DC2691E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{F508C88A-01DC-4D81-9A03-E9861E99A22D}"/>
   </bookViews>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="50">
   <si>
     <t>#</t>
   </si>
@@ -231,6 +231,15 @@
   </si>
   <si>
     <t>Closed</t>
+  </si>
+  <si>
+    <t>Deciding how to structure API for adding budgets. Whether to send included categories over as lists then add them on the backend or split up on front end and make multiple different api calls.</t>
+  </si>
+  <si>
+    <t>SK</t>
+  </si>
+  <si>
+    <t>Make best informed decsion and move forward with building backend.</t>
   </si>
 </sst>
 </file>
@@ -1482,7 +1491,7 @@
   <dimension ref="A1:O60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1548,29 +1557,47 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="47">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
+      <c r="B2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="47">
+        <v>5</v>
+      </c>
+      <c r="F2" s="47">
+        <v>3</v>
+      </c>
       <c r="G2" s="47">
         <f>BRAIDLOG[[#This Row],[Probability]]*BRAIDLOG[[#This Row],[Impact]]</f>
-        <v>0</v>
-      </c>
-      <c r="H2" s="48"/>
+        <v>15</v>
+      </c>
+      <c r="H2" s="48">
+        <v>45182</v>
+      </c>
       <c r="I2" s="48"/>
       <c r="J2" s="47"/>
       <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
+      <c r="L2" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="M2" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="N2" s="47" t="s">
+        <v>48</v>
+      </c>
       <c r="O2" s="2">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1595,7 +1622,7 @@
       <c r="N3" s="47"/>
       <c r="O3" s="2">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1620,7 +1647,7 @@
       <c r="N4" s="51"/>
       <c r="O4" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1645,7 +1672,7 @@
       <c r="N5" s="47"/>
       <c r="O5" s="2">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1670,7 +1697,7 @@
       <c r="N6" s="47"/>
       <c r="O6" s="2">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1695,7 +1722,7 @@
       <c r="N7" s="47"/>
       <c r="O7" s="2">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -1720,7 +1747,7 @@
       <c r="N8" s="51"/>
       <c r="O8" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1745,7 +1772,7 @@
       <c r="N9" s="51"/>
       <c r="O9" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -1770,7 +1797,7 @@
       <c r="N10" s="51"/>
       <c r="O10" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -1795,7 +1822,7 @@
       <c r="N11" s="51"/>
       <c r="O11" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -1820,7 +1847,7 @@
       <c r="N12" s="51"/>
       <c r="O12" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -1845,7 +1872,7 @@
       <c r="N13" s="51"/>
       <c r="O13" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -1870,7 +1897,7 @@
       <c r="N14" s="51"/>
       <c r="O14" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -1895,7 +1922,7 @@
       <c r="N15" s="51"/>
       <c r="O15" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -1920,7 +1947,7 @@
       <c r="N16" s="51"/>
       <c r="O16" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -1945,7 +1972,7 @@
       <c r="N17" s="51"/>
       <c r="O17" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -1970,7 +1997,7 @@
       <c r="N18" s="51"/>
       <c r="O18" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -1995,7 +2022,7 @@
       <c r="N19" s="51"/>
       <c r="O19" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -2020,7 +2047,7 @@
       <c r="N20" s="51"/>
       <c r="O20" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -2045,7 +2072,7 @@
       <c r="N21" s="51"/>
       <c r="O21" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -2070,7 +2097,7 @@
       <c r="N22" s="51"/>
       <c r="O22" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -2093,7 +2120,7 @@
       <c r="N23" s="51"/>
       <c r="O23" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -2116,7 +2143,7 @@
       <c r="N24" s="51"/>
       <c r="O24" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -2139,7 +2166,7 @@
       <c r="N25" s="51"/>
       <c r="O25" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -2162,7 +2189,7 @@
       <c r="N26" s="51"/>
       <c r="O26" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -2185,7 +2212,7 @@
       <c r="N27" s="51"/>
       <c r="O27" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -2208,7 +2235,7 @@
       <c r="N28" s="51"/>
       <c r="O28" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -2231,7 +2258,7 @@
       <c r="N29" s="51"/>
       <c r="O29" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -2254,7 +2281,7 @@
       <c r="N30" s="51"/>
       <c r="O30" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -2277,7 +2304,7 @@
       <c r="N31" s="51"/>
       <c r="O31" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -2300,7 +2327,7 @@
       <c r="N32" s="51"/>
       <c r="O32" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -2323,7 +2350,7 @@
       <c r="N33" s="51"/>
       <c r="O33" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
@@ -2346,7 +2373,7 @@
       <c r="N34" s="51"/>
       <c r="O34" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
@@ -2369,7 +2396,7 @@
       <c r="N35" s="51"/>
       <c r="O35" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
@@ -2392,7 +2419,7 @@
       <c r="N36" s="51"/>
       <c r="O36" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
@@ -2415,7 +2442,7 @@
       <c r="N37" s="51"/>
       <c r="O37" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
@@ -2438,7 +2465,7 @@
       <c r="N38" s="51"/>
       <c r="O38" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
@@ -2461,7 +2488,7 @@
       <c r="N39" s="51"/>
       <c r="O39" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
@@ -2484,7 +2511,7 @@
       <c r="N40" s="51"/>
       <c r="O40" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
@@ -2507,7 +2534,7 @@
       <c r="N41" s="51"/>
       <c r="O41" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
@@ -2530,7 +2557,7 @@
       <c r="N42" s="51"/>
       <c r="O42" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
@@ -2553,7 +2580,7 @@
       <c r="N43" s="51"/>
       <c r="O43" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
@@ -2576,7 +2603,7 @@
       <c r="N44" s="51"/>
       <c r="O44" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
@@ -2599,7 +2626,7 @@
       <c r="N45" s="51"/>
       <c r="O45" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
@@ -2622,7 +2649,7 @@
       <c r="N46" s="51"/>
       <c r="O46" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
@@ -2645,7 +2672,7 @@
       <c r="N47" s="51"/>
       <c r="O47" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
@@ -2668,7 +2695,7 @@
       <c r="N48" s="51"/>
       <c r="O48" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
@@ -2691,7 +2718,7 @@
       <c r="N49" s="51"/>
       <c r="O49" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
@@ -2714,7 +2741,7 @@
       <c r="N50" s="51"/>
       <c r="O50" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
@@ -2737,7 +2764,7 @@
       <c r="N51" s="51"/>
       <c r="O51" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
@@ -2760,7 +2787,7 @@
       <c r="N52" s="51"/>
       <c r="O52" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
@@ -2783,7 +2810,7 @@
       <c r="N53" s="51"/>
       <c r="O53" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
@@ -2806,7 +2833,7 @@
       <c r="N54" s="51"/>
       <c r="O54" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
@@ -2829,7 +2856,7 @@
       <c r="N55" s="51"/>
       <c r="O55" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
@@ -2852,7 +2879,7 @@
       <c r="N56" s="51"/>
       <c r="O56" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
@@ -2875,7 +2902,7 @@
       <c r="N57" s="51"/>
       <c r="O57" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
@@ -2898,7 +2925,7 @@
       <c r="N58" s="51"/>
       <c r="O58" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
@@ -2921,7 +2948,7 @@
       <c r="N59" s="51"/>
       <c r="O59" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
@@ -2944,7 +2971,7 @@
       <c r="N60" s="51"/>
       <c r="O60" s="52">
         <f ca="1">TODAY()-BRAIDLOG[[#This Row],[Date Created]]</f>
-        <v>45119</v>
+        <v>45182</v>
       </c>
     </row>
   </sheetData>
@@ -3647,6 +3674,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003D3EEA9BBC7BDD4FA5B1229800C196A9" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27d6ccb994207a8f84dda17a73ee0918">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5acddd42-0b6b-4e23-9e92-4bfcce45c29d" xmlns:ns3="9382b6d0-5fc1-449f-99fc-f2293a66c4d4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e4c968775d99055df2a5fe78920c7551" ns2:_="" ns3:_="">
     <xsd:import namespace="5acddd42-0b6b-4e23-9e92-4bfcce45c29d"/>
@@ -3863,22 +3905,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{695F9E7E-4D81-48D6-819E-8B10990E01BB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F31D16CB-C141-444E-A63C-574EA86E48EF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41981C6F-3A3E-4DB7-BD7A-F43D3183EFD5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3895,21 +3939,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F31D16CB-C141-444E-A63C-574EA86E48EF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{695F9E7E-4D81-48D6-819E-8B10990E01BB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>